<commit_message>
adding changes to special P port method
</commit_message>
<xml_diff>
--- a/Data Prep Revisi.xlsx
+++ b/Data Prep Revisi.xlsx
@@ -5,18 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Freelancing\Genetic Algorithm Jaringan Kapal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Freelancing\Genetic Algorithm Jaringan Kapal\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4E355A-107A-4FE1-83EA-C490F5A3CA12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9235990-C375-45D0-B739-9F3A622B3E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="2010" windowWidth="20490" windowHeight="10905" firstSheet="1" activeTab="1" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Biaya_Jarak_Teus" sheetId="1" r:id="rId1"/>
     <sheet name="TL_char" sheetId="3" r:id="rId2"/>
     <sheet name="PL_char" sheetId="4" r:id="rId3"/>
     <sheet name="PR_char" sheetId="5" r:id="rId4"/>
+    <sheet name="special_PR" sheetId="6" r:id="rId5"/>
+    <sheet name="wave_status" sheetId="7" r:id="rId6"/>
+    <sheet name="ports" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="121">
   <si>
     <t>P. Kur</t>
   </si>
@@ -373,6 +376,33 @@
   <si>
     <t>ship_char</t>
   </si>
+  <si>
+    <t xml:space="preserve">Werinama </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marlasi </t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>wave_h</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>port_type</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
 </sst>
 </file>
 
@@ -381,7 +411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,8 +442,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +478,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -614,6 +663,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13489,7 +13540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244B3F1C-1EDB-4CF7-97A1-7F6266183B6F}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -18796,4 +18847,1777 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC93771-8FE0-4248-8EEE-4AB295A47998}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C28" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C29" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C31" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851089AA-D5A7-4C66-A791-D07CFCF5E603}">
+  <dimension ref="A1:B77"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K72" sqref="K72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <f ca="1">RAND()*4</f>
+        <v>3.9258182172887786</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" ca="1" si="0">RAND()*4</f>
+        <v>3.7966714822123859</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9309918598091684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.1603439582519046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.691624718310893</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7627253116274106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0051370588183888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5665120580944119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.5612283072997299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.8082281893507184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3256784494396903</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2918960991467205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.9948933782250209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0378802809173662</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7456975036287714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.9516274418116217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.303979374838617</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.7655006305651848</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.54384923533999574</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.491886960706807</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4975404268050556</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.5920587777563213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.327968038814253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.0543644985232787</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.8791400047984061</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0162602653773409</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.88005607722025037</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.6251970458374236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8509208276083839</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6633461260422306</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5191875937343644</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.37396572154301122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.8852890658023669</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.249096272289715</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.45205669438093343</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0291052971168715</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.32222586226903616</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1254628714596508</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99080952680177292</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5126014091245934</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.8258356699326934</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9822697842295836</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9435350259388846</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.2079525413035901</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4448028580442922</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2301560083622411</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2433322260205264</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1957789545871025</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.78536934498491773</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.0943525062856878</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3696406398777889</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.8469069557085298E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.766644701324974</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5904822289844622</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.9996877547739107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5093038067915376</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7425086374208529</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16275601794261751</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.3741046045035459</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4333698029980053</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.6198261388212498</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.149969733366031</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.9221342932557794</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>92</v>
+      </c>
+      <c r="B65">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.6466520515644065</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.8898016362562955</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B77" ca="1" si="1">RAND()*4</f>
+        <v>2.8246071091400435</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84806948985373376</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3611424226646522</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.517227936454002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.2942383653344147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.7682556457143583</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.4821997146280186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38013919002978902</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.5923181810072689</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>52</v>
+      </c>
+      <c r="B76">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7791347997425784</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>62</v>
+      </c>
+      <c r="B77">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.8348237248589951</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E3ABB0-6D15-4E78-AF6E-3E39FC146DC5}">
+  <dimension ref="A1:B92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>37</v>
+      </c>
+      <c r="B83" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>69</v>
+      </c>
+      <c r="B88" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>76</v>
+      </c>
+      <c r="B89" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>50</v>
+      </c>
+      <c r="B90" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>52</v>
+      </c>
+      <c r="B91" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>25</v>
+      </c>
+      <c r="B92" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more debugging shipping system
</commit_message>
<xml_diff>
--- a/Data Prep Revisi.xlsx
+++ b/Data Prep Revisi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Freelancing\Genetic Algorithm Jaringan Kapal\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9235990-C375-45D0-B739-9F3A622B3E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448B7D1D-0850-4E5D-92B7-25E5FE53FA08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Biaya_Jarak_Teus" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="121">
   <si>
     <t>P. Kur</t>
   </si>
@@ -983,7 +983,7 @@
   <dimension ref="A1:CY103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:CY103"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13538,10 +13538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244B3F1C-1EDB-4CF7-97A1-7F6266183B6F}">
-  <dimension ref="A1:K1000"/>
+  <dimension ref="A1:CU1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="CM1" workbookViewId="0">
+      <selection activeCell="CY1" sqref="CY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13550,7 +13550,7 @@
     <col min="27" max="16384" width="14.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>111</v>
       </c>
@@ -13581,8 +13581,272 @@
       <c r="K1" s="12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AS1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="AY1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="BB1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="BC1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="BG1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="BH1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="BI1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="BJ1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="BL1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="BM1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="BN1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO1" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="BP1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="BQ1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="BS1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="BT1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="BV1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BY1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="CA1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="CB1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="CC1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="CD1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="CE1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="CF1" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="CG1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="CH1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="CI1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="CJ1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="CK1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="CL1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="CM1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="CN1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="CO1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="CP1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="CQ1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="CR1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="CS1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="CT1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="CU1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>109</v>
       </c>
@@ -13590,7 +13854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>110</v>
       </c>
@@ -13598,7 +13862,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>102</v>
       </c>
@@ -13629,8 +13893,218 @@
       <c r="K4" s="11">
         <v>32.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="12">
+        <v>181</v>
+      </c>
+      <c r="M4" s="12">
+        <v>126</v>
+      </c>
+      <c r="N4" s="12">
+        <v>129</v>
+      </c>
+      <c r="O4" s="12">
+        <v>164</v>
+      </c>
+      <c r="P4" s="12">
+        <v>181</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>119</v>
+      </c>
+      <c r="R4" s="12">
+        <v>162</v>
+      </c>
+      <c r="S4" s="12">
+        <v>172</v>
+      </c>
+      <c r="T4" s="12">
+        <v>394</v>
+      </c>
+      <c r="U4" s="12">
+        <v>427</v>
+      </c>
+      <c r="V4" s="12">
+        <v>501</v>
+      </c>
+      <c r="W4" s="12">
+        <v>350</v>
+      </c>
+      <c r="X4" s="12">
+        <v>431</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>320</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>437</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>209</v>
+      </c>
+      <c r="AB4" s="12">
+        <v>380</v>
+      </c>
+      <c r="AC4" s="12">
+        <v>513</v>
+      </c>
+      <c r="AD4" s="12">
+        <v>247</v>
+      </c>
+      <c r="AE4" s="12">
+        <v>221</v>
+      </c>
+      <c r="AF4" s="12">
+        <v>155</v>
+      </c>
+      <c r="AG4" s="12">
+        <v>259</v>
+      </c>
+      <c r="AH4" s="12">
+        <v>207</v>
+      </c>
+      <c r="AI4" s="12">
+        <v>178</v>
+      </c>
+      <c r="AJ4" s="12">
+        <v>311</v>
+      </c>
+      <c r="AK4" s="12">
+        <v>302</v>
+      </c>
+      <c r="AL4" s="12">
+        <v>290</v>
+      </c>
+      <c r="AM4" s="12">
+        <v>222</v>
+      </c>
+      <c r="AN4" s="12">
+        <v>207</v>
+      </c>
+      <c r="AO4" s="12">
+        <v>259</v>
+      </c>
+      <c r="AP4" s="12">
+        <v>323</v>
+      </c>
+      <c r="AQ4" s="12">
+        <v>334</v>
+      </c>
+      <c r="AR4" s="12">
+        <v>238</v>
+      </c>
+      <c r="AS4" s="12">
+        <v>208</v>
+      </c>
+      <c r="AT4" s="12">
+        <v>244</v>
+      </c>
+      <c r="AU4" s="12">
+        <v>300</v>
+      </c>
+      <c r="AV4" s="12">
+        <v>253</v>
+      </c>
+      <c r="AW4" s="12">
+        <v>311</v>
+      </c>
+      <c r="AX4" s="12">
+        <v>315</v>
+      </c>
+      <c r="AY4" s="12">
+        <v>221</v>
+      </c>
+      <c r="AZ4" s="12">
+        <v>282</v>
+      </c>
+      <c r="BA4" s="12">
+        <v>185</v>
+      </c>
+      <c r="BB4" s="12">
+        <v>440</v>
+      </c>
+      <c r="BC4" s="12">
+        <v>325</v>
+      </c>
+      <c r="BD4" s="12">
+        <v>382</v>
+      </c>
+      <c r="BE4" s="12">
+        <v>436</v>
+      </c>
+      <c r="BF4" s="12">
+        <v>293</v>
+      </c>
+      <c r="BG4" s="12">
+        <v>480</v>
+      </c>
+      <c r="BH4" s="12">
+        <v>366</v>
+      </c>
+      <c r="BI4" s="12">
+        <v>310</v>
+      </c>
+      <c r="BJ4" s="12">
+        <v>384</v>
+      </c>
+      <c r="BK4" s="12">
+        <v>322</v>
+      </c>
+      <c r="BL4" s="12">
+        <v>383</v>
+      </c>
+      <c r="BM4" s="12">
+        <v>238</v>
+      </c>
+      <c r="BN4" s="12">
+        <v>352</v>
+      </c>
+      <c r="BO4" s="12">
+        <v>322</v>
+      </c>
+      <c r="BP4" s="12">
+        <v>261</v>
+      </c>
+      <c r="BQ4" s="12">
+        <v>296</v>
+      </c>
+      <c r="BR4" s="12">
+        <v>245</v>
+      </c>
+      <c r="BS4" s="12">
+        <v>244</v>
+      </c>
+      <c r="BT4" s="12">
+        <v>248</v>
+      </c>
+      <c r="BU4" s="12">
+        <v>191</v>
+      </c>
+      <c r="BV4" s="12">
+        <v>221</v>
+      </c>
+      <c r="BW4" s="12">
+        <v>180</v>
+      </c>
+      <c r="BX4" s="12">
+        <v>283</v>
+      </c>
+      <c r="BY4" s="12">
+        <v>156</v>
+      </c>
+      <c r="BZ4" s="12">
+        <v>163</v>
+      </c>
+      <c r="CA4" s="12">
+        <v>220</v>
+      </c>
+      <c r="CB4" s="12">
+        <v>189</v>
+      </c>
+      <c r="CC4" s="12">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>103</v>
       </c>
@@ -13661,8 +14135,218 @@
       <c r="K5" s="11">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="12">
+        <v>24</v>
+      </c>
+      <c r="M5" s="12">
+        <v>24</v>
+      </c>
+      <c r="N5" s="12">
+        <v>24</v>
+      </c>
+      <c r="O5" s="12">
+        <v>24</v>
+      </c>
+      <c r="P5" s="12">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>24</v>
+      </c>
+      <c r="R5" s="12">
+        <v>24</v>
+      </c>
+      <c r="S5" s="12">
+        <v>24</v>
+      </c>
+      <c r="T5" s="12">
+        <v>24</v>
+      </c>
+      <c r="U5" s="12">
+        <v>24</v>
+      </c>
+      <c r="V5" s="12">
+        <v>24</v>
+      </c>
+      <c r="W5" s="12">
+        <v>24</v>
+      </c>
+      <c r="X5" s="12">
+        <v>24</v>
+      </c>
+      <c r="Y5" s="12">
+        <v>24</v>
+      </c>
+      <c r="Z5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AA5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AB5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AC5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AD5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AE5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AF5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AG5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AH5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AI5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AJ5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AK5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AL5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AM5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AN5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AO5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AP5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AQ5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AR5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AS5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AT5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AU5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AV5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AW5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AX5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AY5" s="12">
+        <v>24</v>
+      </c>
+      <c r="AZ5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BA5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BB5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BC5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BD5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BE5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BF5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BG5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BH5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BI5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BJ5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BK5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BL5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BM5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BN5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BO5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BP5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BQ5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BR5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BS5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BT5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BU5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BV5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BW5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BX5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BY5" s="12">
+        <v>24</v>
+      </c>
+      <c r="BZ5" s="12">
+        <v>24</v>
+      </c>
+      <c r="CA5" s="12">
+        <v>24</v>
+      </c>
+      <c r="CB5" s="12">
+        <v>24</v>
+      </c>
+      <c r="CC5" s="12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>104</v>
       </c>
@@ -13693,8 +14377,218 @@
       <c r="K6" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="12">
+        <v>5</v>
+      </c>
+      <c r="M6" s="12">
+        <v>5</v>
+      </c>
+      <c r="N6" s="12">
+        <v>5</v>
+      </c>
+      <c r="O6" s="12">
+        <v>5</v>
+      </c>
+      <c r="P6" s="12">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>5</v>
+      </c>
+      <c r="R6" s="12">
+        <v>5</v>
+      </c>
+      <c r="S6" s="12">
+        <v>5</v>
+      </c>
+      <c r="T6" s="12">
+        <v>5</v>
+      </c>
+      <c r="U6" s="12">
+        <v>5</v>
+      </c>
+      <c r="V6" s="12">
+        <v>5</v>
+      </c>
+      <c r="W6" s="12">
+        <v>5</v>
+      </c>
+      <c r="X6" s="12">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="12">
+        <v>5</v>
+      </c>
+      <c r="Z6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AB6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AC6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AE6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AF6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AG6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AI6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AJ6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AK6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AL6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AM6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AO6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AP6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AQ6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AR6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AS6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AT6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AU6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AV6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AW6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AX6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AY6" s="12">
+        <v>5</v>
+      </c>
+      <c r="AZ6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BA6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BB6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BC6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BD6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BF6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BG6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BH6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BI6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BJ6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BK6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BL6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BM6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BN6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BO6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BP6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BQ6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BR6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BS6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BT6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BU6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BV6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BW6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BX6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BY6" s="12">
+        <v>5</v>
+      </c>
+      <c r="BZ6" s="12">
+        <v>5</v>
+      </c>
+      <c r="CA6" s="12">
+        <v>5</v>
+      </c>
+      <c r="CB6" s="12">
+        <v>5</v>
+      </c>
+      <c r="CC6" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>105</v>
       </c>
@@ -13725,8 +14619,218 @@
       <c r="K7" s="11">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="12">
+        <v>3</v>
+      </c>
+      <c r="M7" s="12">
+        <v>3</v>
+      </c>
+      <c r="N7" s="12">
+        <v>3</v>
+      </c>
+      <c r="O7" s="12">
+        <v>3</v>
+      </c>
+      <c r="P7" s="12">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>3</v>
+      </c>
+      <c r="R7" s="12">
+        <v>3</v>
+      </c>
+      <c r="S7" s="12">
+        <v>3</v>
+      </c>
+      <c r="T7" s="12">
+        <v>3</v>
+      </c>
+      <c r="U7" s="12">
+        <v>3</v>
+      </c>
+      <c r="V7" s="12">
+        <v>3</v>
+      </c>
+      <c r="W7" s="12">
+        <v>3</v>
+      </c>
+      <c r="X7" s="12">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AD7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AE7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AF7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AG7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AH7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AI7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AJ7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AK7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AL7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AM7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AN7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AO7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AP7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AQ7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AR7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AS7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AT7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AU7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AV7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AW7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AX7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AY7" s="12">
+        <v>3</v>
+      </c>
+      <c r="AZ7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BA7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BB7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BC7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BD7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BE7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BF7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BG7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BH7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BI7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BJ7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BK7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BL7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BM7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BN7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BO7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BP7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BQ7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BR7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BS7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BT7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BU7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BV7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BW7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BX7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BY7" s="12">
+        <v>3</v>
+      </c>
+      <c r="BZ7" s="12">
+        <v>3</v>
+      </c>
+      <c r="CA7" s="12">
+        <v>3</v>
+      </c>
+      <c r="CB7" s="12">
+        <v>3</v>
+      </c>
+      <c r="CC7" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>106</v>
       </c>
@@ -13757,8 +14861,218 @@
       <c r="K8" s="11">
         <v>20000</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="12">
+        <v>700</v>
+      </c>
+      <c r="M8" s="12">
+        <v>700</v>
+      </c>
+      <c r="N8" s="12">
+        <v>700</v>
+      </c>
+      <c r="O8" s="12">
+        <v>700</v>
+      </c>
+      <c r="P8" s="12">
+        <v>700</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>700</v>
+      </c>
+      <c r="R8" s="12">
+        <v>700</v>
+      </c>
+      <c r="S8" s="12">
+        <v>700</v>
+      </c>
+      <c r="T8" s="12">
+        <v>700</v>
+      </c>
+      <c r="U8" s="12">
+        <v>700</v>
+      </c>
+      <c r="V8" s="12">
+        <v>700</v>
+      </c>
+      <c r="W8" s="12">
+        <v>700</v>
+      </c>
+      <c r="X8" s="12">
+        <v>700</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>700</v>
+      </c>
+      <c r="Z8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AA8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AB8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AC8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AD8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AE8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AF8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AG8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AH8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AI8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AJ8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AK8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AL8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AM8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AN8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AO8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AP8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AQ8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AR8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AS8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AT8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AU8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AV8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AW8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AX8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AY8" s="12">
+        <v>700</v>
+      </c>
+      <c r="AZ8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BA8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BB8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BC8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BD8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BE8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BF8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BG8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BH8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BI8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BJ8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BK8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BL8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BM8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BN8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BO8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BP8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BQ8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BR8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BS8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BT8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BU8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BV8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BW8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BX8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BY8" s="12">
+        <v>700</v>
+      </c>
+      <c r="BZ8" s="12">
+        <v>700</v>
+      </c>
+      <c r="CA8" s="12">
+        <v>700</v>
+      </c>
+      <c r="CB8" s="12">
+        <v>700</v>
+      </c>
+      <c r="CC8" s="12">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>107</v>
       </c>
@@ -13789,8 +15103,218 @@
       <c r="K9" s="11">
         <v>375</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="M9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="N9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="O9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="P9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="R9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="S9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="T9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="U9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="V9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="W9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="X9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="Y9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="Z9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AA9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AB9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AC9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AD9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AE9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AF9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AG9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AH9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AI9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AJ9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AK9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AL9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AM9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AN9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AO9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AP9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AQ9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AR9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AS9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AT9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AU9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AV9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AW9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AX9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AY9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="AZ9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BA9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BB9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BC9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BD9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BE9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BF9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BG9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BH9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BI9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BJ9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BK9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BL9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BM9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BN9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BO9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BP9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BQ9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BR9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BS9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BT9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BU9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BV9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BW9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BX9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BY9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="BZ9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="CA9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="CB9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="CC9" s="12">
+        <v>22.916666666666668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>108</v>
       </c>
@@ -13820,6 +15344,216 @@
       </c>
       <c r="K10" s="11">
         <v>15000</v>
+      </c>
+      <c r="L10" s="12">
+        <v>900</v>
+      </c>
+      <c r="M10" s="12">
+        <v>900</v>
+      </c>
+      <c r="N10" s="12">
+        <v>900</v>
+      </c>
+      <c r="O10" s="12">
+        <v>900</v>
+      </c>
+      <c r="P10" s="12">
+        <v>900</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>900</v>
+      </c>
+      <c r="R10" s="12">
+        <v>900</v>
+      </c>
+      <c r="S10" s="12">
+        <v>900</v>
+      </c>
+      <c r="T10" s="12">
+        <v>900</v>
+      </c>
+      <c r="U10" s="12">
+        <v>900</v>
+      </c>
+      <c r="V10" s="12">
+        <v>900</v>
+      </c>
+      <c r="W10" s="12">
+        <v>900</v>
+      </c>
+      <c r="X10" s="12">
+        <v>900</v>
+      </c>
+      <c r="Y10" s="12">
+        <v>900</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AA10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AB10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AC10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AD10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AE10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AF10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AG10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AH10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AI10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AJ10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AK10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AL10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AM10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AN10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AO10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AP10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AQ10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AR10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AS10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AT10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AU10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AV10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AW10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AX10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AY10" s="12">
+        <v>900</v>
+      </c>
+      <c r="AZ10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BA10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BB10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BC10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BD10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BE10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BF10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BG10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BH10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BI10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BJ10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BK10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BL10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BM10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BN10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BO10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BP10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BQ10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BR10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BS10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BT10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BU10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BV10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BW10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BX10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BY10" s="12">
+        <v>900</v>
+      </c>
+      <c r="BZ10" s="12">
+        <v>900</v>
+      </c>
+      <c r="CA10" s="12">
+        <v>900</v>
+      </c>
+      <c r="CB10" s="12">
+        <v>900</v>
+      </c>
+      <c r="CC10" s="12">
+        <v>900</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14813,7 +16547,7 @@
   <dimension ref="A1:J996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="K1" sqref="K1:CW10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16052,10 +17786,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B556AD0-CF09-4AD2-90F5-FEC655BECA7C}">
-  <dimension ref="A1:CL1000"/>
+  <dimension ref="A1:CO1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="CO1" sqref="C1:CO10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16065,7 +17799,7 @@
     <col min="73" max="16384" width="14.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="B1" s="11" t="s">
         <v>111</v>
@@ -16334,8 +18068,17 @@
       <c r="CL1" s="13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="CM1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="CN1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="CO1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:93" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>109</v>
       </c>
@@ -16343,7 +18086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:93" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>110</v>
       </c>
@@ -16351,7 +18094,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>102</v>
       </c>
@@ -16567,7 +18310,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>103</v>
       </c>
@@ -16783,7 +18526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>104</v>
       </c>
@@ -16999,7 +18742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>105</v>
       </c>
@@ -17215,7 +18958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>106</v>
       </c>
@@ -17431,7 +19174,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>107</v>
       </c>
@@ -17647,7 +19390,7 @@
         <v>22.916666666666668</v>
       </c>
     </row>
-    <row r="10" spans="1:90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>108</v>
       </c>
@@ -19188,7 +20931,7 @@
       </c>
       <c r="B2">
         <f ca="1">RAND()*4</f>
-        <v>3.9258182172887786</v>
+        <v>3.8657462865316594</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -19197,7 +20940,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" ca="1" si="0">RAND()*4</f>
-        <v>3.7966714822123859</v>
+        <v>3.815263671976679</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -19206,7 +20949,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9309918598091684</v>
+        <v>0.52030655107817569</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -19215,7 +20958,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1603439582519046</v>
+        <v>0.16184890859374734</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -19224,7 +20967,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.691624718310893</v>
+        <v>0.73150698891926824</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -19233,7 +20976,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7627253116274106</v>
+        <v>3.0704645603309157</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -19242,7 +20985,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0051370588183888</v>
+        <v>3.5834059803763569</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -19251,7 +20994,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5665120580944119</v>
+        <v>1.8060941483055801</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -19260,7 +21003,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5612283072997299</v>
+        <v>1.5379672044156538</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -19269,7 +21012,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8082281893507184</v>
+        <v>1.7667435587169642</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -19278,7 +21021,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3256784494396903</v>
+        <v>1.4343973669428758</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -19287,7 +21030,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2918960991467205</v>
+        <v>0.23633153363062753</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -19296,7 +21039,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9948933782250209</v>
+        <v>3.6587498703673806</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -19305,7 +21048,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0378802809173662</v>
+        <v>2.4543638633930911</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -19314,7 +21057,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7456975036287714</v>
+        <v>3.7988105839121928</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -19323,7 +21066,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9516274418116217</v>
+        <v>1.5122446193232157</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -19332,7 +21075,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>3.303979374838617</v>
+        <v>2.1190036140470272</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -19341,7 +21084,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7655006305651848</v>
+        <v>0.93730024278991619</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -19350,7 +21093,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54384923533999574</v>
+        <v>2.0122836755658451</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -19359,7 +21102,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>2.491886960706807</v>
+        <v>2.6213596840296254</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -19368,7 +21111,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4975404268050556</v>
+        <v>0.77891550508762508</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -19377,7 +21120,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5920587777563213</v>
+        <v>0.63818541533430295</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -19386,7 +21129,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>1.327968038814253</v>
+        <v>0.33815827489270411</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -19395,7 +21138,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0543644985232787</v>
+        <v>1.6791663762256062</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -19404,7 +21147,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8791400047984061</v>
+        <v>3.8317187581732814</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -19413,7 +21156,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0162602653773409</v>
+        <v>0.19106843409612528</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -19422,7 +21165,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88005607722025037</v>
+        <v>0.16255611110338952</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -19431,7 +21174,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6251970458374236</v>
+        <v>3.3421166612231574</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -19440,7 +21183,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8509208276083839</v>
+        <v>3.9876995382584766</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -19449,7 +21192,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6633461260422306</v>
+        <v>0.90527082716142315</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -19458,7 +21201,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5191875937343644</v>
+        <v>0.34162480522140859</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -19467,7 +21210,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37396572154301122</v>
+        <v>2.781502155661002</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -19476,7 +21219,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8852890658023669</v>
+        <v>2.4875932189690215</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -19485,7 +21228,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>3.249096272289715</v>
+        <v>1.3313597641427748</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -19494,7 +21237,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45205669438093343</v>
+        <v>2.4722045925321732</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -19503,7 +21246,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0291052971168715</v>
+        <v>0.40795783615196246</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -19512,7 +21255,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32222586226903616</v>
+        <v>0.31521699156455396</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -19521,7 +21264,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1254628714596508</v>
+        <v>0.63956129178590748</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -19530,7 +21273,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99080952680177292</v>
+        <v>1.2752661647397421</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -19539,7 +21282,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5126014091245934</v>
+        <v>2.048790268354121</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -19548,7 +21291,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8258356699326934</v>
+        <v>1.1231046728119747</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -19557,7 +21300,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9822697842295836</v>
+        <v>2.3596725775917768</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -19566,7 +21309,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9435350259388846</v>
+        <v>2.7952315484475982</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -19575,7 +21318,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2079525413035901</v>
+        <v>2.8850145344487963</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -19584,7 +21327,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4448028580442922</v>
+        <v>0.53224250513349336</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -19593,7 +21336,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2301560083622411</v>
+        <v>3.1969248726241624</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -19602,7 +21345,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2433322260205264</v>
+        <v>1.456966318237586</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -19611,7 +21354,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1957789545871025</v>
+        <v>1.1990687991688507</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -19620,7 +21363,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78536934498491773</v>
+        <v>3.3634790718295808</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -19629,7 +21372,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0943525062856878</v>
+        <v>1.4994041960329834</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -19638,7 +21381,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3696406398777889</v>
+        <v>2.4350191965139873</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -19647,7 +21390,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8469069557085298E-2</v>
+        <v>1.3070722784086515</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -19656,7 +21399,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="0"/>
-        <v>3.766644701324974</v>
+        <v>3.2804260165878114</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -19665,7 +21408,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5904822289844622</v>
+        <v>1.8232949173329329</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -19674,7 +21417,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9996877547739107</v>
+        <v>3.3973829521557652</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -19683,7 +21426,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5093038067915376</v>
+        <v>0.75923451678366227</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -19692,7 +21435,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7425086374208529</v>
+        <v>1.7952891615480326</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -19701,7 +21444,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16275601794261751</v>
+        <v>0.76231066126782876</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -19710,7 +21453,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3741046045035459</v>
+        <v>0.25403133742653639</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -19719,7 +21462,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4333698029980053</v>
+        <v>2.2551251588229446</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -19728,7 +21471,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6198261388212498</v>
+        <v>1.0048520536604078</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -19737,7 +21480,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="0"/>
-        <v>2.149969733366031</v>
+        <v>3.6653295746677452</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -19746,7 +21489,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9221342932557794</v>
+        <v>2.8686198167205004</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -19755,7 +21498,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6466520515644065</v>
+        <v>2.0714734190881487</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -19764,7 +21507,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8898016362562955</v>
+        <v>2.8577144753306989</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -19773,7 +21516,7 @@
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B77" ca="1" si="1">RAND()*4</f>
-        <v>2.8246071091400435</v>
+        <v>3.7436654835108065</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -19782,7 +21525,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84806948985373376</v>
+        <v>3.7269447809951668</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -19791,7 +21534,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3611424226646522</v>
+        <v>1.0360802243508633</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -19800,7 +21543,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="1"/>
-        <v>3.517227936454002</v>
+        <v>2.6586461511763524</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -19809,7 +21552,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2942383653344147</v>
+        <v>1.9160502659892842</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -19818,7 +21561,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7682556457143583</v>
+        <v>2.0217072319628002</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -19827,7 +21570,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4821997146280186</v>
+        <v>2.7451586673628268</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -19836,7 +21579,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38013919002978902</v>
+        <v>3.6030401438717057</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -19845,7 +21588,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5923181810072689</v>
+        <v>0.80809561543920605</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -19854,7 +21597,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7791347997425784</v>
+        <v>1.9518309655925141</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -19863,7 +21606,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8348237248589951</v>
+        <v>1.1187303101986363</v>
       </c>
     </row>
   </sheetData>
@@ -19875,8 +21618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E3ABB0-6D15-4E78-AF6E-3E39FC146DC5}">
   <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Simulation done 1 recommit
making sure nothing is missed
</commit_message>
<xml_diff>
--- a/Data Prep Revisi.xlsx
+++ b/Data Prep Revisi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Freelancing\Genetic Algorithm Jaringan Kapal\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2C3951-39BA-44D3-BA29-90A184F1738A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D368678-15EE-4F2A-9453-26717AC44D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{4237FA56-EEE5-40CD-9C70-C83858DBAEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Biaya_Jarak_Teus" sheetId="1" r:id="rId1"/>
@@ -381,10 +381,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +425,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -608,11 +616,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -639,8 +648,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{F7153D30-257E-4796-9251-C996041D116F}"/>
   </cellStyles>
@@ -956,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9E6091-9B8B-49E8-ACBA-74D06FEDF945}">
   <dimension ref="A1:CP93"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
@@ -11497,8 +11525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244B3F1C-1EDB-4CF7-97A1-7F6266183B6F}">
   <dimension ref="A1:CK1000"/>
   <sheetViews>
-    <sheetView topLeftCell="BJ1" workbookViewId="0">
-      <selection activeCell="BJ1" sqref="BJ1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11799,34 +11827,34 @@
       <c r="D4" s="12">
         <v>45</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="21">
         <v>40</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="21">
         <v>48</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="21">
         <v>35</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="21">
         <v>40</v>
       </c>
-      <c r="I4" s="12">
-        <v>20</v>
-      </c>
-      <c r="J4" s="12">
-        <v>45</v>
-      </c>
-      <c r="K4" s="11">
+      <c r="I4" s="22">
+        <v>10</v>
+      </c>
+      <c r="J4" s="20">
+        <v>5</v>
+      </c>
+      <c r="K4" s="23">
         <v>32.5</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="21">
         <v>181</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="21">
         <v>126</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="21">
         <v>129</v>
       </c>
       <c r="O4" s="12">
@@ -12041,34 +12069,34 @@
       <c r="D5" s="12">
         <v>120</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="21">
         <v>120</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="21">
         <v>120</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="21">
         <v>120</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="21">
         <v>120</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="22">
         <v>8</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="24">
         <v>4</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="23">
         <v>6</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="21">
         <v>24</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="21">
         <v>24</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="21">
         <v>24</v>
       </c>
       <c r="O5" s="12">
@@ -12283,34 +12311,34 @@
       <c r="D6" s="12">
         <v>4</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="21">
         <v>4</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="21">
         <v>4</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="21">
         <v>4</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="21">
         <v>4</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="22">
         <v>2</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="24">
         <v>2</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="23">
         <v>2</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="21">
         <v>5</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="21">
         <v>5</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="21">
         <v>5</v>
       </c>
       <c r="O6" s="12">
@@ -12525,34 +12553,35 @@
       <c r="D7" s="12">
         <v>3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="21">
         <v>3</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="21">
         <v>3</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="21">
         <v>3</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="21">
         <v>3</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="22">
         <v>72</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="24">
+        <f t="shared" ref="J7" si="0">3*24</f>
         <v>72</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="23">
         <v>72</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="21">
         <v>3</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="21">
         <v>3</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="21">
         <v>3</v>
       </c>
       <c r="O7" s="12">
@@ -12767,34 +12796,34 @@
       <c r="D8" s="12">
         <v>20000</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="21">
         <v>20000</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="21">
         <v>20000</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="21">
         <v>20000</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="21">
         <v>20000</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="22">
         <v>20000</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="24">
         <v>20000</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="23">
         <v>20000</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="21">
         <v>700</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="21">
         <v>700</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="21">
         <v>700</v>
       </c>
       <c r="O8" s="12">
@@ -13009,34 +13038,35 @@
       <c r="D9" s="12">
         <v>183.33333333333334</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="21">
         <v>183.33333333333334</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="21">
         <v>183.33333333333334</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="21">
         <v>183.33333333333334</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="21">
         <v>183.33333333333334</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="22">
         <v>375</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="24">
+        <f>9000/24</f>
         <v>375</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="23">
         <v>375</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="21">
         <v>22.916666666666668</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="21">
         <v>22.916666666666668</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="21">
         <v>22.916666666666668</v>
       </c>
       <c r="O9" s="12">
@@ -13251,34 +13281,34 @@
       <c r="D10" s="12">
         <v>15000</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="21">
         <v>15000</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="21">
         <v>15000</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="21">
         <v>15000</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="21">
         <v>15000</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="25">
         <v>15000</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="24">
         <v>15000</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="23">
         <v>15000</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="21">
         <v>900</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="21">
         <v>900</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="21">
         <v>900</v>
       </c>
       <c r="O10" s="12">
@@ -13482,6 +13512,9 @@
       <c r="CC10" s="12">
         <v>900</v>
       </c>
+    </row>
+    <row r="13" spans="1:89" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="12"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14474,7 +14507,7 @@
   <dimension ref="A1:J996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14532,6 +14565,9 @@
       <c r="A4" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="C4" s="11">
+        <v>5</v>
+      </c>
       <c r="D4" s="12">
         <v>20</v>
       </c>
@@ -14558,6 +14594,9 @@
       <c r="A5" s="12" t="s">
         <v>88</v>
       </c>
+      <c r="C5" s="11">
+        <v>8</v>
+      </c>
       <c r="D5" s="12">
         <v>8</v>
       </c>
@@ -14584,6 +14623,9 @@
       <c r="A6" s="12" t="s">
         <v>89</v>
       </c>
+      <c r="C6" s="11">
+        <v>2</v>
+      </c>
       <c r="D6" s="12">
         <v>2</v>
       </c>
@@ -14610,6 +14652,9 @@
       <c r="A7" s="12" t="s">
         <v>90</v>
       </c>
+      <c r="C7" s="11">
+        <v>72</v>
+      </c>
       <c r="D7" s="12">
         <v>72</v>
       </c>
@@ -14636,6 +14681,9 @@
       <c r="A8" s="12" t="s">
         <v>91</v>
       </c>
+      <c r="C8" s="11">
+        <v>20000</v>
+      </c>
       <c r="D8" s="12">
         <v>20000</v>
       </c>
@@ -14662,6 +14710,9 @@
       <c r="A9" s="12" t="s">
         <v>92</v>
       </c>
+      <c r="C9" s="11">
+        <v>375</v>
+      </c>
       <c r="D9" s="12">
         <v>375</v>
       </c>
@@ -14688,6 +14739,9 @@
       <c r="A10" s="12" t="s">
         <v>93</v>
       </c>
+      <c r="C10" s="11">
+        <v>15000</v>
+      </c>
       <c r="D10" s="12">
         <v>15000</v>
       </c>
@@ -14718,9 +14772,6 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
@@ -18496,7 +18547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC93771-8FE0-4248-8EEE-4AB295A47998}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -18811,8 +18862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851089AA-D5A7-4C66-A791-D07CFCF5E603}">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18831,7 +18882,7 @@
       </c>
       <c r="B2">
         <f ca="1">RAND()*4</f>
-        <v>3.704430428941492</v>
+        <v>3.6437498617413544</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -18840,7 +18891,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" ca="1" si="0">RAND()*4</f>
-        <v>3.1042111290104097</v>
+        <v>3.4005766583459391</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -18849,7 +18900,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8655017364817748</v>
+        <v>1.7170425428539193</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -18858,7 +18909,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1426637115658518</v>
+        <v>1.5746348658102036</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -18867,7 +18918,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85060349187252537</v>
+        <v>2.3273877448532647</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -18876,7 +18927,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49741560294897358</v>
+        <v>1.7717744974652936</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -18885,7 +18936,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82068410810307979</v>
+        <v>2.884122475362132</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -18894,7 +18945,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.551373852206023</v>
+        <v>3.9154208802339694</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -18903,7 +18954,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8662190316722085</v>
+        <v>0.56341844133846042</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -18912,7 +18963,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3161589482961031</v>
+        <v>0.77709961110061032</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -18921,7 +18972,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89989319858700467</v>
+        <v>0.70762040609410004</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -18930,7 +18981,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8872222339775582</v>
+        <v>1.6895085151234635</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -18939,7 +18990,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9207047201939589</v>
+        <v>1.9542207009789667</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -18948,7 +18999,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6746764244853587E-2</v>
+        <v>2.2181903901504878</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -18957,7 +19008,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61465256978898974</v>
+        <v>2.8180602783590372</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -18966,7 +19017,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1424445091934139</v>
+        <v>0.56275469569669623</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -18975,7 +19026,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95057732564993014</v>
+        <v>1.4784052613168193</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -18984,7 +19035,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9392553483000192</v>
+        <v>3.1569349800993192</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -18993,7 +19044,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1122170215198199</v>
+        <v>3.3555358665685295</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -19002,7 +19053,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2645536204862688</v>
+        <v>0.36686165446288976</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -19011,7 +19062,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5852124970643007</v>
+        <v>0.60076790705608207</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -19020,7 +19071,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8435826677395921</v>
+        <v>2.9626851346692002</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -19029,7 +19080,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91089866472046044</v>
+        <v>2.5133023363768476</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -19038,7 +19089,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>8.1160023381809054E-2</v>
+        <v>2.1200094384351891</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -19047,7 +19098,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11029646146272176</v>
+        <v>0.93970280610458667</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -19056,7 +19107,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1500902468280878</v>
+        <v>0.99217558899168212</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -19065,7 +19116,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1460648494395271</v>
+        <v>3.9885659687030959</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -19074,7 +19125,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6096037892637192</v>
+        <v>1.9959310569637423</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -19083,7 +19134,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2789786805973815</v>
+        <v>3.840389218711282</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -19092,7 +19143,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0378275560073495</v>
+        <v>3.3778657488915118</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -19101,7 +19152,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22763087257246228</v>
+        <v>3.5712697281946273</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -19110,7 +19161,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5992217275107268</v>
+        <v>3.5916004618797164</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -19119,7 +19170,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1367599903268708</v>
+        <v>2.7984874324778115</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -19128,7 +19179,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0736973583869971</v>
+        <v>3.1724065857810224</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -19137,7 +19188,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63610612263489141</v>
+        <v>3.4079472822695283</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -19146,7 +19197,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90079002368929961</v>
+        <v>0.3242745240180267</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -19155,7 +19206,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2500052871224296</v>
+        <v>3.2087484791038414</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -19164,7 +19215,7 @@
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9064735783563806</v>
+        <v>1.1716828194924185</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -19173,7 +19224,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6321432714187565</v>
+        <v>1.6943662029848934</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -19182,7 +19233,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4890866106068912</v>
+        <v>0.67852000925618094</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -19191,7 +19242,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68428964589895225</v>
+        <v>0.51517745514838564</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -19200,7 +19251,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0660241692618402</v>
+        <v>0.86466438161388304</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -19209,7 +19260,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4065590097920699</v>
+        <v>1.9349795266598511</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -19218,7 +19269,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30797249709407826</v>
+        <v>1.3965061316399541</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -19227,7 +19278,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>1.82265137868584</v>
+        <v>0.39102354390104876</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -19236,7 +19287,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46349599690691745</v>
+        <v>3.995846191757666</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -19245,7 +19296,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3466023549507349</v>
+        <v>3.9725228119299785</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -19254,7 +19305,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5231454920612251</v>
+        <v>2.2922746231556586</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -19263,7 +19314,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0944943384583978</v>
+        <v>0.54299172453701816</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -19272,7 +19323,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1770469899465716</v>
+        <v>2.5306796664564386</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -19281,7 +19332,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5663558321615132</v>
+        <v>2.8173542830303306</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -19290,7 +19341,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7476945014348777</v>
+        <v>1.1240367860775327</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -19299,7 +19350,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3155982463697136</v>
+        <v>1.8310691427726304</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -19308,7 +19359,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39546610876711163</v>
+        <v>0.69656116089276576</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -19317,7 +19368,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7537407634643052</v>
+        <v>3.0602062822856486</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -19326,7 +19377,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66791252848019944</v>
+        <v>1.3938397686809543</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -19335,7 +19386,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1799274185010691</v>
+        <v>3.303052408860025</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -19344,7 +19395,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3098609798937</v>
+        <v>2.0880694450728519</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -19353,7 +19404,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6411136369545676</v>
+        <v>1.7210115720973165</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -19362,7 +19413,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21721663459009877</v>
+        <v>3.4626581128947431</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -19371,7 +19422,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84958772028851071</v>
+        <v>2.8913424887209298</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -19380,7 +19431,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6392785146420965</v>
+        <v>2.0018952017902309</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -19389,7 +19440,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2758490774095042</v>
+        <v>2.8401756441278776</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -19398,7 +19449,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6620106662955139</v>
+        <v>0.10725073043552902</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -19407,7 +19458,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2447496110438845</v>
+        <v>3.3754805733800448</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -19416,7 +19467,7 @@
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B77" ca="1" si="1">RAND()*4</f>
-        <v>3.2642294389008821</v>
+        <v>2.1186801527317973</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -19425,7 +19476,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6116136786385225</v>
+        <v>3.8060971047379044</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -19434,7 +19485,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13159170472681669</v>
+        <v>9.1446063712973924E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -19443,7 +19494,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="1"/>
-        <v>3.6192242849279901</v>
+        <v>0.542004651679727</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -19452,7 +19503,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76979632574060952</v>
+        <v>1.7613888633153314</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -19461,7 +19512,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3901959849076881</v>
+        <v>3.2776304107041008</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -19470,7 +19521,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2168583533990982</v>
+        <v>2.8819765572189122</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -19479,7 +19530,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2030482056611906</v>
+        <v>1.8877458121980841</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -19488,7 +19539,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="1"/>
-        <v>2.996432014713434</v>
+        <v>2.4852610227896501</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -19497,7 +19548,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0123739628166408</v>
+        <v>2.2348723751013493</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -19506,7 +19557,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2648151301483757</v>
+        <v>1.1499612584876391</v>
       </c>
     </row>
   </sheetData>
@@ -19518,8 +19569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E3ABB0-6D15-4E78-AF6E-3E39FC146DC5}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>